<commit_message>
Add battery and power control
</commit_message>
<xml_diff>
--- a/Default Configuration/Project Outputs for Data-Logger-Prototyping-Board/BOM/BOM_PartType-Data-Logger-Prototyping-Board.xlsx
+++ b/Default Configuration/Project Outputs for Data-Logger-Prototyping-Board/BOM/BOM_PartType-Data-Logger-Prototyping-Board.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ADB10BE-79BA-433F-ACE4-F2E39B74DE25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="13395" windowHeight="10545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13635" windowHeight="13890" xr2:uid="{99A0DCB9-680E-4E2A-97AF-A9DD51E9D4E5}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Data-Logger-Protot" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
   <si>
     <t>Designator</t>
   </si>
@@ -28,7 +34,7 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C7, C10</t>
+    <t>C1, C2, C3, C6, C7, C8, C9, C10, C13, C14</t>
   </si>
   <si>
     <t>100nF, 0603</t>
@@ -37,22 +43,31 @@
     <t>Capacitor 0603</t>
   </si>
   <si>
-    <t>C6, C8</t>
-  </si>
-  <si>
-    <t>22pF, 0603</t>
-  </si>
-  <si>
-    <t>C9</t>
+    <t>C4, C5, C15, C16, C18</t>
+  </si>
+  <si>
+    <t>4.7uF, 0603</t>
+  </si>
+  <si>
+    <t>C11, C19</t>
+  </si>
+  <si>
+    <t>10uF, 0603</t>
+  </si>
+  <si>
+    <t>C12</t>
   </si>
   <si>
     <t>4.7nF, 0603</t>
   </si>
   <si>
-    <t>C11, C12, C13</t>
-  </si>
-  <si>
-    <t>10uF, 0603</t>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>33uF, 1.69mR, 0805 (C2012X5R1A336M125AC)</t>
+  </si>
+  <si>
+    <t>Capacitor 0805</t>
   </si>
   <si>
     <t>D1</t>
@@ -61,6 +76,36 @@
     <t>D3V3X4U10LP</t>
   </si>
   <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>MBR1020VL</t>
+  </si>
+  <si>
+    <t>SOD-123</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Red LED, 0603</t>
+  </si>
+  <si>
+    <t>LED 0603</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Yellow LED, 0603</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>Green LED, 0603</t>
+  </si>
+  <si>
     <t>J1</t>
   </si>
   <si>
@@ -85,25 +130,43 @@
     <t>MOLEX-47309-2851</t>
   </si>
   <si>
-    <t>JP1</t>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>4UCON-20404</t>
+  </si>
+  <si>
+    <t>JP1, JP2, JP3, JP4</t>
   </si>
   <si>
     <t>Jumper 2-way</t>
   </si>
   <si>
-    <t>JP2</t>
-  </si>
-  <si>
-    <t>Jumper 3-way</t>
-  </si>
-  <si>
-    <t>Q1</t>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>3.3uH, 25.2mR (MSS5131-332MLB)</t>
+  </si>
+  <si>
+    <t>MSS5131</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3</t>
   </si>
   <si>
     <t>SIA437DJ-T1-GE3</t>
   </si>
   <si>
-    <t>R1, R7, R8, R9, R10, R11, R12</t>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>RN1901FETE85LF</t>
+  </si>
+  <si>
+    <t>SOT-666</t>
+  </si>
+  <si>
+    <t>R1, R5, R6, R7, R8, R9, R10, R12, R14</t>
   </si>
   <si>
     <t>10kR, 0603</t>
@@ -112,31 +175,46 @@
     <t>Resistor 0603</t>
   </si>
   <si>
-    <t>R2, R4</t>
-  </si>
-  <si>
-    <t>22R, 0603</t>
-  </si>
-  <si>
-    <t>R3, R5</t>
+    <t>R2, R4, R16, R19, R20</t>
   </si>
   <si>
     <t>470R, 0603</t>
   </si>
   <si>
-    <t>R6</t>
+    <t>R3</t>
   </si>
   <si>
     <t>1MR, 0603</t>
   </si>
   <si>
-    <t>S1</t>
+    <t>R11, R13</t>
+  </si>
+  <si>
+    <t>4.7kR, 0603</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>1kR, 0603</t>
+  </si>
+  <si>
+    <t>R17, R18</t>
+  </si>
+  <si>
+    <t>100kR, 0603</t>
+  </si>
+  <si>
+    <t>S1, S2</t>
+  </si>
+  <si>
+    <t>FSM4JAH</t>
   </si>
   <si>
     <t>FSM4JHX</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32, TP33</t>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24, TP25, TP26</t>
   </si>
   <si>
     <t>Test Point</t>
@@ -157,34 +235,58 @@
     <t>U2</t>
   </si>
   <si>
-    <t>ADP3338AKCZ-3.3-RL</t>
-  </si>
-  <si>
-    <t>SOT-223</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ASTMTXK-32.768kHz-LG-T</t>
-  </si>
-  <si>
-    <t>ASTMTXK</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
-    <t>ABM8-24.000MHZ-B2-T</t>
-  </si>
-  <si>
-    <t>ABM8</t>
+    <t>LP5907SNX-3.1</t>
+  </si>
+  <si>
+    <t>X2SON</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>ASTMLPA-24.000MHz-LJ-E-T</t>
+  </si>
+  <si>
+    <t>ASTMLPA</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>M41T62LC6F</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>24AA32AT-I/OT</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>MCP73830LT-0AAI/MYY</t>
+  </si>
+  <si>
+    <t>TDFN-6 2x2mm</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>TPS63001DRC</t>
+  </si>
+  <si>
+    <t>VSON-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -258,6 +360,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -273,44 +378,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -338,14 +443,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -373,6 +495,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -384,172 +523,148 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A5202B-9DC4-4C41-A30D-952C7E9FB651}">
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,7 +695,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -594,7 +709,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -608,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -622,7 +737,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -642,245 +757,413 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B19" s="3">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="3">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>